<commit_message>
added panacea to test data
</commit_message>
<xml_diff>
--- a/taxonomic key data.xlsx
+++ b/taxonomic key data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Software\TaxKeyGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DEAD52-825C-455D-866F-545C696C5F07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5168F87B-B3BB-47A0-9347-107CAD1FD4DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="825" windowWidth="26310" windowHeight="18255" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
+    <workbookView xWindow="6075" yWindow="825" windowWidth="26310" windowHeight="18255" activeTab="1" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>.</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>panacea</t>
   </si>
 </sst>
 </file>
@@ -472,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF502AD-4408-4993-BE91-9B79E0A99B48}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC15929-3CC2-4C58-A610-B698FFC4555C}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="A1:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -806,19 +809,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>1.2</v>
       </c>
       <c r="C3">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D3">
-        <v>3.1</v>
+        <v>3.3</v>
       </c>
       <c r="E3">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
       <c r="F3">
         <v>5.2</v>
@@ -841,6 +844,26 @@
         <v>4.2</v>
       </c>
       <c r="F4">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>1.2</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+      <c r="D5">
+        <v>3.1</v>
+      </c>
+      <c r="E5">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F5">
         <v>5.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating data with images
</commit_message>
<xml_diff>
--- a/taxonomic key data.xlsx
+++ b/taxonomic key data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Software\TaxKeyGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58F5A30-F369-448F-BD42-B1E589BCF41A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E413B7-F0F3-4AA6-91D4-0A6C361015AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="750" windowWidth="26310" windowHeight="18255" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
+    <workbookView xWindow="7935" yWindow="105" windowWidth="26310" windowHeight="18255" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
-  <si>
-    <t>.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Trait</t>
   </si>
@@ -85,9 +82,6 @@
     <t>H-groove color</t>
   </si>
   <si>
-    <t>H-groove is same color as the rest of the carapace</t>
-  </si>
-  <si>
     <t>H-groove is silver-gray</t>
   </si>
   <si>
@@ -121,13 +115,49 @@
     <t>panacea</t>
   </si>
   <si>
-    <t>M_minax.jpg|Red markings on joints of claw and limb.</t>
-  </si>
-  <si>
-    <t>L_pugilator02.jpg|.</t>
-  </si>
-  <si>
-    <t>L_pugilator01.jpg|H-groove is silver-gray.</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>1.1.png|Narrow-front, with eyestalks close together.</t>
+  </si>
+  <si>
+    <t>1.2.png|Broad-front with eyestalks farther apart.</t>
+  </si>
+  <si>
+    <t>2.1.jpg|Carapace predominantly a solid single color.</t>
+  </si>
+  <si>
+    <t>2.2.jpg|Carapace multiple colors.</t>
+  </si>
+  <si>
+    <t>5.1.jpg|Red markings on joints of claw and limb.</t>
+  </si>
+  <si>
+    <t>H-groove is same color as (or not distinct from) the rest of the carapace</t>
+  </si>
+  <si>
+    <t>4.1.jpg|H-groove is similar color to carapace.</t>
+  </si>
+  <si>
+    <t>4.2a.jpg|H-groove is silver-gray.||4.2b.jpg|H-groove is silver-gray.</t>
+  </si>
+  <si>
+    <t>4.3a.jpg|H-groove is rusty-red.||4.3b.jpg|H-groove is rusty-red.</t>
+  </si>
+  <si>
+    <t>5.2.jpg|Joints lack distinctive red markings.</t>
+  </si>
+  <si>
+    <t>3.1a.jpg|Medium-to-dark blue carapace.||3.1b.jpg|Medium-to-dark blue carapace.</t>
+  </si>
+  <si>
+    <t>3.2.jpg|silver-tan carapace.</t>
+  </si>
+  <si>
+    <t>L_pugilator02.jpg|White/cream carapace with purple blotches.</t>
   </si>
 </sst>
 </file>
@@ -485,7 +515,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,22 +529,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -522,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>10</v>
@@ -531,10 +561,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -542,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -551,10 +581,10 @@
         <v>1.2</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -562,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -571,10 +601,10 @@
         <v>2.1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -582,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -591,10 +621,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,7 +632,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -611,10 +641,10 @@
         <v>3.1</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,7 +652,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -631,10 +661,10 @@
         <v>3.2</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -642,7 +672,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -651,10 +681,10 @@
         <v>3.3</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,7 +692,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -671,10 +701,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,7 +712,7 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -691,10 +721,10 @@
         <v>4.2</v>
       </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +732,7 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -711,10 +741,10 @@
         <v>4.3</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -722,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -731,10 +761,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -742,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -751,10 +781,10 @@
         <v>5.2</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -764,10 +794,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADC15929-3CC2-4C58-A610-B698FFC4555C}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,27 +808,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="126.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2">
         <v>1.2</v>
@@ -818,7 +848,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>1.2</v>
@@ -838,7 +868,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <v>1.2</v>
@@ -858,7 +888,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>1.2</v>
@@ -873,6 +903,46 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="F5">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>1.2</v>
+      </c>
+      <c r="C6">
+        <v>2.1</v>
+      </c>
+      <c r="D6">
+        <v>3.1</v>
+      </c>
+      <c r="E6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F6">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>1.2</v>
+      </c>
+      <c r="C7">
+        <v>2.1</v>
+      </c>
+      <c r="D7">
+        <v>3.1</v>
+      </c>
+      <c r="E7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F7">
         <v>5.2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
starting footnote output support
</commit_message>
<xml_diff>
--- a/taxonomic key data.xlsx
+++ b/taxonomic key data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Software\TaxKeyGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2098AE22-56DF-4BFD-B864-BAE32CB8AD07}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248A908-25C0-404C-9908-54520D055466}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="1" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="356">
   <si>
     <t>Trait</t>
   </si>
@@ -1099,6 +1099,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -1517,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF502AD-4408-4993-BE91-9B79E0A99B48}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1589,7 +1592,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>355</v>
       </c>
       <c r="E4" t="s">
         <v>28</v>
@@ -1725,7 +1728,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>355</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
@@ -1876,7 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{000B03AE-DDB5-42CA-B0F1-F1BD4626B09E}">
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
restoring and udpating some data
</commit_message>
<xml_diff>
--- a/taxonomic key data.xlsx
+++ b/taxonomic key data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Software\TaxKeyGen\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\Software\TaxKeyGen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4248A908-25C0-404C-9908-54520D055466}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04B8A03-DEAC-4D63-A7F5-B8F8A83A88E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
+    <workbookView xWindow="11700" yWindow="1725" windowWidth="26310" windowHeight="18255" xr2:uid="{10F64F7F-A08F-47A2-ACFC-F3D7F9FF1593}"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1843" uniqueCount="359">
   <si>
     <t>Trait</t>
   </si>
@@ -1101,7 +1101,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Front Breadth: Test test test and more test.</t>
+  </si>
+  <si>
+    <t>Carapace Color: This is just a test to see if the system is working. Something about carapace color. Blah blah blah blah blah.</t>
+  </si>
+  <si>
+    <t>Claw Color: Perhaps another test will be useful.</t>
+  </si>
+  <si>
+    <t>Outer Manus Color: Let's try yet another test.</t>
   </si>
 </sst>
 </file>
@@ -1521,16 +1530,16 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1547,7 +1556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1558,13 +1567,13 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>355</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1581,7 +1590,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1592,13 +1601,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1632,7 +1641,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1649,7 +1658,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1666,7 +1675,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1683,7 +1692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1700,7 +1709,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1717,7 +1726,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1728,13 +1737,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1785,7 +1794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1813,13 +1822,13 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>358</v>
       </c>
       <c r="E17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1836,7 +1845,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1853,7 +1862,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1872,6 +1881,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1880,15 +1890,15 @@
   <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="70.44140625" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1899,7 +1909,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -1910,7 +1920,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -1921,7 +1931,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2.1</v>
       </c>
@@ -1932,7 +1942,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.2000000000000002</v>
       </c>
@@ -1943,7 +1953,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.2999999999999998</v>
       </c>
@@ -1954,7 +1964,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.1</v>
       </c>
@@ -1965,7 +1975,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.2</v>
       </c>
@@ -1976,7 +1986,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3.3</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3.4</v>
       </c>
@@ -1998,7 +2008,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3.5</v>
       </c>
@@ -2009,7 +2019,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3.6</v>
       </c>
@@ -2020,7 +2030,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3.7</v>
       </c>
@@ -2031,7 +2041,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3.8</v>
       </c>
@@ -2042,7 +2052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3.9</v>
       </c>
@@ -2053,7 +2063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>337</v>
       </c>
@@ -2064,7 +2074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4.0999999999999996</v>
       </c>
@@ -2075,7 +2085,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4.2</v>
       </c>
@@ -2086,7 +2096,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4.3</v>
       </c>
@@ -2097,7 +2107,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5.0999999999999996</v>
       </c>
@@ -2108,7 +2118,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5.2</v>
       </c>
@@ -2119,7 +2129,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6.1</v>
       </c>
@@ -2130,7 +2140,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6.2</v>
       </c>
@@ -2141,7 +2151,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7.1</v>
       </c>
@@ -2152,7 +2162,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7.2</v>
       </c>
@@ -2163,7 +2173,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8.1</v>
       </c>
@@ -2174,7 +2184,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8.1999999999999993</v>
       </c>
@@ -2185,7 +2195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8.3000000000000007</v>
       </c>
@@ -2196,7 +2206,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8.4</v>
       </c>
@@ -2207,7 +2217,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8.5</v>
       </c>
@@ -2218,7 +2228,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8.6</v>
       </c>
@@ -2229,7 +2239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9.1</v>
       </c>
@@ -2240,7 +2250,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9.1999999999999993</v>
       </c>
@@ -2251,7 +2261,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10.1</v>
       </c>
@@ -2262,7 +2272,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10.199999999999999</v>
       </c>
@@ -2273,7 +2283,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10.3</v>
       </c>
@@ -2284,7 +2294,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10.4</v>
       </c>
@@ -2295,7 +2305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10.5</v>
       </c>
@@ -2306,7 +2316,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11.1</v>
       </c>
@@ -2317,7 +2327,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>11.2</v>
       </c>
@@ -2328,7 +2338,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12.1</v>
       </c>
@@ -2339,7 +2349,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12.2</v>
       </c>
@@ -2350,7 +2360,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12.3</v>
       </c>
@@ -2361,7 +2371,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13.1</v>
       </c>
@@ -2372,7 +2382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>13.2</v>
       </c>
@@ -2383,7 +2393,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>14.1</v>
       </c>
@@ -2394,7 +2404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14.2</v>
       </c>
@@ -2405,7 +2415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>15.1</v>
       </c>
@@ -2416,7 +2426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>15.2</v>
       </c>
@@ -2427,7 +2437,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15.3</v>
       </c>
@@ -2438,7 +2448,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15.4</v>
       </c>
@@ -2449,7 +2459,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15.5</v>
       </c>
@@ -2460,7 +2470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>16.100000000000001</v>
       </c>
@@ -2471,7 +2481,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>16.2</v>
       </c>
@@ -2482,7 +2492,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>16.3</v>
       </c>
@@ -2493,7 +2503,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>16.399999999999999</v>
       </c>
@@ -2504,7 +2514,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>16.5</v>
       </c>
@@ -2515,7 +2525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>16.600000000000001</v>
       </c>
@@ -2526,7 +2536,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>16.7</v>
       </c>
@@ -2537,7 +2547,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>17.100000000000001</v>
       </c>
@@ -2548,7 +2558,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>17.2</v>
       </c>
@@ -2559,7 +2569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>18.100000000000001</v>
       </c>
@@ -2570,7 +2580,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>18.2</v>
       </c>
@@ -2581,7 +2591,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>18.3</v>
       </c>
@@ -2592,7 +2602,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>19.100000000000001</v>
       </c>
@@ -2603,7 +2613,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>19.2</v>
       </c>
@@ -2627,15 +2637,15 @@
       <selection activeCell="A4" sqref="A1:T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="9" width="5.6640625" style="1"/>
-    <col min="11" max="13" width="5.6640625" style="1"/>
-    <col min="15" max="15" width="5.6640625" style="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="9" width="5.7109375" style="1"/>
+    <col min="11" max="13" width="5.7109375" style="1"/>
+    <col min="15" max="15" width="5.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -2697,7 +2707,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -2759,7 +2769,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -2821,7 +2831,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -2883,7 +2893,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2945,7 +2955,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -3007,7 +3017,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -3069,7 +3079,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -3131,7 +3141,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -3193,7 +3203,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -3255,7 +3265,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>73</v>
       </c>
@@ -3317,7 +3327,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -3379,7 +3389,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
@@ -3441,7 +3451,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -3503,7 +3513,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>259</v>
       </c>
@@ -3565,7 +3575,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>260</v>
       </c>
@@ -3627,7 +3637,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>261</v>
       </c>
@@ -3689,7 +3699,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>262</v>
       </c>
@@ -3751,7 +3761,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>263</v>
       </c>
@@ -3813,7 +3823,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>264</v>
       </c>
@@ -3875,7 +3885,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>265</v>
       </c>
@@ -3937,7 +3947,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>266</v>
       </c>
@@ -3999,7 +4009,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>267</v>
       </c>
@@ -4061,7 +4071,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>268</v>
       </c>
@@ -4123,7 +4133,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>269</v>
       </c>
@@ -4185,7 +4195,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>270</v>
       </c>
@@ -4247,7 +4257,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>271</v>
       </c>
@@ -4309,7 +4319,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>157</v>
       </c>
@@ -4371,7 +4381,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>245</v>
       </c>
@@ -4433,7 +4443,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>183</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>107</v>
       </c>
@@ -4557,7 +4567,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>151</v>
       </c>
@@ -4619,7 +4629,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>158</v>
       </c>
@@ -4681,7 +4691,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>246</v>
       </c>
@@ -4743,7 +4753,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>184</v>
       </c>
@@ -4805,7 +4815,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>108</v>
       </c>
@@ -4867,7 +4877,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>152</v>
       </c>
@@ -4929,7 +4939,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>77</v>
       </c>
@@ -4949,7 +4959,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>79</v>
       </c>
@@ -4969,7 +4979,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>81</v>
       </c>
@@ -4989,7 +4999,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>83</v>
       </c>
@@ -5009,7 +5019,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>85</v>
       </c>
@@ -5029,7 +5039,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>87</v>
       </c>
@@ -5049,7 +5059,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>89</v>
       </c>
@@ -5069,7 +5079,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>91</v>
       </c>
@@ -5089,7 +5099,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>93</v>
       </c>
@@ -5109,7 +5119,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>95</v>
       </c>
@@ -5129,7 +5139,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>97</v>
       </c>
@@ -5149,7 +5159,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>99</v>
       </c>
@@ -5169,7 +5179,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>101</v>
       </c>
@@ -5189,7 +5199,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>103</v>
       </c>
@@ -5209,7 +5219,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>105</v>
       </c>
@@ -5229,7 +5239,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>109</v>
       </c>
@@ -5249,7 +5259,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>111</v>
       </c>
@@ -5269,7 +5279,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>113</v>
       </c>
@@ -5289,7 +5299,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>115</v>
       </c>
@@ -5309,7 +5319,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>117</v>
       </c>
@@ -5329,7 +5339,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>119</v>
       </c>
@@ -5349,7 +5359,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>121</v>
       </c>
@@ -5369,7 +5379,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>123</v>
       </c>
@@ -5389,7 +5399,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>125</v>
       </c>
@@ -5409,7 +5419,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>127</v>
       </c>
@@ -5429,7 +5439,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>129</v>
       </c>
@@ -5449,7 +5459,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>131</v>
       </c>
@@ -5469,7 +5479,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>133</v>
       </c>
@@ -5489,7 +5499,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>135</v>
       </c>
@@ -5509,7 +5519,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>137</v>
       </c>
@@ -5529,7 +5539,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>139</v>
       </c>
@@ -5549,7 +5559,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>141</v>
       </c>
@@ -5569,7 +5579,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>143</v>
       </c>
@@ -5589,7 +5599,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>145</v>
       </c>
@@ -5609,7 +5619,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>147</v>
       </c>
@@ -5629,7 +5639,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>149</v>
       </c>
@@ -5649,7 +5659,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>153</v>
       </c>
@@ -5669,7 +5679,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>155</v>
       </c>
@@ -5689,7 +5699,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>159</v>
       </c>
@@ -5709,7 +5719,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>161</v>
       </c>
@@ -5729,7 +5739,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>163</v>
       </c>
@@ -5749,7 +5759,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>165</v>
       </c>
@@ -5769,7 +5779,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>167</v>
       </c>
@@ -5789,7 +5799,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>169</v>
       </c>
@@ -5809,7 +5819,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>171</v>
       </c>
@@ -5829,7 +5839,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>173</v>
       </c>
@@ -5849,7 +5859,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>175</v>
       </c>
@@ -5869,7 +5879,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>177</v>
       </c>
@@ -5889,7 +5899,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>179</v>
       </c>
@@ -5909,7 +5919,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>181</v>
       </c>
@@ -5929,7 +5939,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>185</v>
       </c>
@@ -5949,7 +5959,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>187</v>
       </c>
@@ -5969,7 +5979,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>189</v>
       </c>
@@ -5989,7 +5999,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>191</v>
       </c>
@@ -6009,7 +6019,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>193</v>
       </c>
@@ -6029,7 +6039,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>195</v>
       </c>
@@ -6049,7 +6059,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>197</v>
       </c>
@@ -6069,7 +6079,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>199</v>
       </c>
@@ -6089,7 +6099,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>201</v>
       </c>
@@ -6109,7 +6119,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>203</v>
       </c>
@@ -6129,7 +6139,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>205</v>
       </c>
@@ -6149,7 +6159,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
         <v>207</v>
       </c>
@@ -6169,7 +6179,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>209</v>
       </c>
@@ -6189,7 +6199,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
         <v>211</v>
       </c>
@@ -6209,7 +6219,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
         <v>213</v>
       </c>
@@ -6229,7 +6239,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
         <v>215</v>
       </c>
@@ -6249,7 +6259,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>217</v>
       </c>
@@ -6269,7 +6279,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>219</v>
       </c>
@@ -6289,7 +6299,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>221</v>
       </c>
@@ -6309,7 +6319,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>223</v>
       </c>
@@ -6329,7 +6339,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>225</v>
       </c>
@@ -6352,7 +6362,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>227</v>
       </c>
@@ -6372,7 +6382,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>229</v>
       </c>
@@ -6392,7 +6402,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>231</v>
       </c>
@@ -6412,7 +6422,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>233</v>
       </c>
@@ -6432,7 +6442,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="5" t="s">
         <v>235</v>
       </c>
@@ -6452,7 +6462,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>237</v>
       </c>
@@ -6472,7 +6482,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>239</v>
       </c>
@@ -6492,7 +6502,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="5" t="s">
         <v>241</v>
       </c>
@@ -6512,7 +6522,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="5" t="s">
         <v>243</v>
       </c>
@@ -6532,7 +6542,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="5" t="s">
         <v>247</v>
       </c>
@@ -6552,7 +6562,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="5" t="s">
         <v>249</v>
       </c>
@@ -6572,7 +6582,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="5" t="s">
         <v>251</v>
       </c>
@@ -6592,7 +6602,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="5" t="s">
         <v>253</v>
       </c>
@@ -6612,7 +6622,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>255</v>
       </c>
@@ -6632,7 +6642,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="5" t="s">
         <v>257</v>
       </c>
@@ -6652,7 +6662,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="5" t="s">
         <v>78</v>
       </c>
@@ -6696,7 +6706,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="5" t="s">
         <v>80</v>
       </c>
@@ -6740,7 +6750,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>82</v>
       </c>
@@ -6784,7 +6794,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="5" t="s">
         <v>84</v>
       </c>
@@ -6828,7 +6838,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="5" t="s">
         <v>86</v>
       </c>
@@ -6872,7 +6882,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="5" t="s">
         <v>88</v>
       </c>
@@ -6916,7 +6926,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="5" t="s">
         <v>90</v>
       </c>
@@ -6960,7 +6970,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="5" t="s">
         <v>92</v>
       </c>
@@ -7004,7 +7014,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="5" t="s">
         <v>94</v>
       </c>
@@ -7048,7 +7058,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="5" t="s">
         <v>96</v>
       </c>
@@ -7092,7 +7102,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="5" t="s">
         <v>98</v>
       </c>
@@ -7136,7 +7146,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>100</v>
       </c>
@@ -7180,7 +7190,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="5" t="s">
         <v>102</v>
       </c>
@@ -7224,7 +7234,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="5" t="s">
         <v>104</v>
       </c>
@@ -7268,7 +7278,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="5" t="s">
         <v>106</v>
       </c>
@@ -7312,7 +7322,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="5" t="s">
         <v>110</v>
       </c>
@@ -7356,7 +7366,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="5" t="s">
         <v>112</v>
       </c>
@@ -7400,7 +7410,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="5" t="s">
         <v>114</v>
       </c>
@@ -7444,7 +7454,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="5" t="s">
         <v>116</v>
       </c>
@@ -7488,7 +7498,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>118</v>
       </c>
@@ -7532,7 +7542,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" s="5" t="s">
         <v>120</v>
       </c>
@@ -7576,7 +7586,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="5" t="s">
         <v>122</v>
       </c>
@@ -7620,7 +7630,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>124</v>
       </c>
@@ -7664,7 +7674,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="5" t="s">
         <v>126</v>
       </c>
@@ -7708,7 +7718,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" s="5" t="s">
         <v>128</v>
       </c>
@@ -7752,7 +7762,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
         <v>130</v>
       </c>
@@ -7796,7 +7806,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" s="5" t="s">
         <v>132</v>
       </c>
@@ -7840,7 +7850,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" s="5" t="s">
         <v>134</v>
       </c>
@@ -7884,7 +7894,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="5" t="s">
         <v>136</v>
       </c>
@@ -7928,7 +7938,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="5" t="s">
         <v>138</v>
       </c>
@@ -7972,7 +7982,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" s="5" t="s">
         <v>140</v>
       </c>
@@ -8016,7 +8026,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="5" t="s">
         <v>142</v>
       </c>
@@ -8060,7 +8070,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="5" t="s">
         <v>144</v>
       </c>
@@ -8104,7 +8114,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="5" t="s">
         <v>146</v>
       </c>
@@ -8148,7 +8158,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>148</v>
       </c>
@@ -8192,7 +8202,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="5" t="s">
         <v>150</v>
       </c>
@@ -8236,7 +8246,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="5" t="s">
         <v>154</v>
       </c>
@@ -8280,7 +8290,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>156</v>
       </c>
@@ -8324,7 +8334,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="5" t="s">
         <v>160</v>
       </c>
@@ -8368,7 +8378,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>162</v>
       </c>
@@ -8412,7 +8422,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="5" t="s">
         <v>164</v>
       </c>
@@ -8456,7 +8466,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="5" t="s">
         <v>166</v>
       </c>
@@ -8500,7 +8510,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="5" t="s">
         <v>168</v>
       </c>
@@ -8544,7 +8554,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="5" t="s">
         <v>170</v>
       </c>
@@ -8588,7 +8598,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>172</v>
       </c>
@@ -8632,7 +8642,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="5" t="s">
         <v>174</v>
       </c>
@@ -8676,7 +8686,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>176</v>
       </c>
@@ -8720,7 +8730,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="5" t="s">
         <v>178</v>
       </c>
@@ -8764,7 +8774,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="5" t="s">
         <v>180</v>
       </c>
@@ -8808,7 +8818,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
         <v>182</v>
       </c>
@@ -8852,7 +8862,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" s="5" t="s">
         <v>186</v>
       </c>
@@ -8896,7 +8906,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" s="5" t="s">
         <v>188</v>
       </c>
@@ -8940,7 +8950,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
         <v>190</v>
       </c>
@@ -8984,7 +8994,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="5" t="s">
         <v>192</v>
       </c>
@@ -9028,7 +9038,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="5" t="s">
         <v>194</v>
       </c>
@@ -9072,7 +9082,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" s="5" t="s">
         <v>196</v>
       </c>
@@ -9116,7 +9126,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>198</v>
       </c>
@@ -9160,7 +9170,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" s="5" t="s">
         <v>200</v>
       </c>
@@ -9204,7 +9214,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" s="5" t="s">
         <v>202</v>
       </c>
@@ -9248,7 +9258,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" s="5" t="s">
         <v>204</v>
       </c>
@@ -9292,7 +9302,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>206</v>
       </c>
@@ -9336,7 +9346,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" s="5" t="s">
         <v>208</v>
       </c>
@@ -9380,7 +9390,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" s="5" t="s">
         <v>210</v>
       </c>
@@ -9424,7 +9434,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" s="5" t="s">
         <v>212</v>
       </c>
@@ -9468,7 +9478,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" s="5" t="s">
         <v>214</v>
       </c>
@@ -9512,7 +9522,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" s="5" t="s">
         <v>216</v>
       </c>
@@ -9556,7 +9566,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
         <v>218</v>
       </c>
@@ -9600,7 +9610,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A194" s="5" t="s">
         <v>220</v>
       </c>
@@ -9644,7 +9654,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195" s="5" t="s">
         <v>222</v>
       </c>
@@ -9688,7 +9698,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
         <v>224</v>
       </c>
@@ -9732,7 +9742,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="5" t="s">
         <v>226</v>
       </c>
@@ -9776,7 +9786,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198" s="5" t="s">
         <v>228</v>
       </c>
@@ -9820,7 +9830,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="5" t="s">
         <v>230</v>
       </c>
@@ -9864,7 +9874,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" s="5" t="s">
         <v>232</v>
       </c>
@@ -9908,7 +9918,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201" s="5" t="s">
         <v>234</v>
       </c>
@@ -9952,7 +9962,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202" s="5" t="s">
         <v>236</v>
       </c>
@@ -9996,7 +10006,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203" s="5" t="s">
         <v>238</v>
       </c>
@@ -10040,7 +10050,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204" s="5" t="s">
         <v>240</v>
       </c>
@@ -10084,7 +10094,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="205" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A205" s="5" t="s">
         <v>242</v>
       </c>
@@ -10128,7 +10138,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="206" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A206" s="5" t="s">
         <v>244</v>
       </c>
@@ -10172,7 +10182,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="207" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A207" s="5" t="s">
         <v>248</v>
       </c>
@@ -10216,7 +10226,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="208" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A208" s="5" t="s">
         <v>250</v>
       </c>
@@ -10260,7 +10270,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="209" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A209" s="5" t="s">
         <v>252</v>
       </c>
@@ -10304,7 +10314,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="210" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A210" s="5" t="s">
         <v>254</v>
       </c>
@@ -10348,7 +10358,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="211" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A211" s="5" t="s">
         <v>256</v>
       </c>
@@ -10392,7 +10402,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="212" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A212" s="5" t="s">
         <v>258</v>
       </c>
@@ -10463,19 +10473,19 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="76.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="76.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -10495,7 +10505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10515,7 +10525,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -10535,7 +10545,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -10555,7 +10565,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -10575,7 +10585,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -10595,7 +10605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -10615,7 +10625,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -10635,7 +10645,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -10655,7 +10665,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -10675,7 +10685,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -10695,7 +10705,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -10715,7 +10725,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -10735,7 +10745,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -10755,7 +10765,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -10775,7 +10785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -10795,7 +10805,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -10815,7 +10825,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -10835,7 +10845,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -10855,7 +10865,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -10875,7 +10885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>5</v>
       </c>
@@ -10895,7 +10905,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6</v>
       </c>
@@ -10915,7 +10925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>6</v>
       </c>
@@ -10935,7 +10945,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7</v>
       </c>
@@ -10955,7 +10965,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -10975,7 +10985,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -10995,7 +11005,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8</v>
       </c>
@@ -11015,7 +11025,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -11035,7 +11045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8</v>
       </c>
@@ -11055,7 +11065,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
@@ -11075,7 +11085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8</v>
       </c>
@@ -11095,7 +11105,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -11115,7 +11125,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9</v>
       </c>
@@ -11135,7 +11145,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>10</v>
       </c>
@@ -11155,7 +11165,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>10</v>
       </c>
@@ -11175,7 +11185,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>10</v>
       </c>
@@ -11195,7 +11205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>10</v>
       </c>
@@ -11215,7 +11225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>10</v>
       </c>
@@ -11235,7 +11245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>11</v>
       </c>
@@ -11255,7 +11265,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>11</v>
       </c>
@@ -11275,7 +11285,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>12</v>
       </c>
@@ -11295,7 +11305,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>12</v>
       </c>
@@ -11315,7 +11325,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>12</v>
       </c>
@@ -11335,7 +11345,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>13</v>
       </c>
@@ -11355,7 +11365,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>13</v>
       </c>
@@ -11375,7 +11385,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>14</v>
       </c>
@@ -11395,7 +11405,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>14</v>
       </c>
@@ -11415,7 +11425,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>15</v>
       </c>
@@ -11435,7 +11445,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>15</v>
       </c>
@@ -11455,7 +11465,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>15</v>
       </c>
@@ -11475,7 +11485,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>15</v>
       </c>
@@ -11495,7 +11505,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>15</v>
       </c>
@@ -11515,7 +11525,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>16</v>
       </c>
@@ -11535,7 +11545,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>16</v>
       </c>
@@ -11555,7 +11565,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>16</v>
       </c>
@@ -11575,7 +11585,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>16</v>
       </c>
@@ -11595,7 +11605,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>16</v>
       </c>
@@ -11615,7 +11625,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>16</v>
       </c>
@@ -11635,7 +11645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>16</v>
       </c>
@@ -11655,7 +11665,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>17</v>
       </c>
@@ -11675,7 +11685,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>17</v>
       </c>
@@ -11695,7 +11705,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>18</v>
       </c>
@@ -11715,7 +11725,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>18</v>
       </c>
@@ -11735,7 +11745,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>18</v>
       </c>
@@ -11755,7 +11765,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>19</v>
       </c>
@@ -11775,7 +11785,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>19</v>
       </c>

</xml_diff>